<commit_message>
remove names of concepts and relations just for the Braga-demo.
</commit_message>
<xml_diff>
--- a/Braga/Braga.xlsx
+++ b/Braga/Braga.xlsx
@@ -11,14 +11,13 @@
     <sheet name="Relations" sheetId="3" r:id="rId2"/>
     <sheet name="Rules" sheetId="4" r:id="rId3"/>
     <sheet name="Compositions" sheetId="8" r:id="rId4"/>
-    <sheet name="Intersections" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>[Concept]</t>
   </si>
@@ -26,9 +25,6 @@
     <t>Concept</t>
   </si>
   <si>
-    <t>isa</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -81,12 +77,6 @@
   </si>
   <si>
     <t>Composition</t>
-  </si>
-  <si>
-    <t>[Intersection]</t>
-  </si>
-  <si>
-    <t>Intersection</t>
   </si>
   <si>
     <t>lhsTerm</t>
@@ -463,9 +453,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="E8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -474,21 +519,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -496,114 +541,35 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -626,35 +592,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -668,7 +634,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -679,160 +645,123 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
esthetic refinements on Braga
</commit_message>
<xml_diff>
--- a/Braga/Braga.xlsx
+++ b/Braga/Braga.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>[Concept]</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Concept</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>[Relation]</t>
   </si>
   <si>
@@ -35,9 +32,6 @@
   </si>
   <si>
     <t>r</t>
-  </si>
-  <si>
-    <t>Identifier</t>
   </si>
   <si>
     <t>A</t>
@@ -453,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C5"/>
+      <selection activeCell="A6" sqref="A6:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -464,39 +458,29 @@
     <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="E8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="E9" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -509,7 +493,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -519,18 +503,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -541,35 +525,35 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +566,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -592,35 +576,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -634,7 +618,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G11"/>
+      <selection activeCell="A4" sqref="A4:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -645,123 +629,123 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduced interesting error messages
</commit_message>
<xml_diff>
--- a/Braga/Braga.xlsx
+++ b/Braga/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>[Concept]</t>
   </si>
@@ -110,6 +110,27 @@
   </si>
   <si>
     <t>s;r</t>
+  </si>
+  <si>
+    <t>undeclared</t>
+  </si>
+  <si>
+    <t>undeclared = s;t</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>v = w</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -490,10 +511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -556,6 +577,33 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -563,18 +611,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -585,7 +635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -596,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -604,6 +654,28 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -617,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C11"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -661,13 +733,13 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="E4" s="1" t="s">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
used in Braga presentation
</commit_message>
<xml_diff>
--- a/Braga/Braga.xlsx
+++ b/Braga/Braga.xlsx
@@ -4,23 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Concepts" sheetId="1" r:id="rId1"/>
-    <sheet name="Relations" sheetId="3" r:id="rId2"/>
-    <sheet name="Rules" sheetId="4" r:id="rId3"/>
-    <sheet name="Compositions" sheetId="8" r:id="rId4"/>
+    <sheet name="Relations" sheetId="3" r:id="rId1"/>
+    <sheet name="Rules" sheetId="4" r:id="rId2"/>
+    <sheet name="Compositions" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
-  <si>
-    <t>[Concept]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>Concept</t>
   </si>
@@ -115,9 +111,6 @@
     <t>undeclared</t>
   </si>
   <si>
-    <t>undeclared = s;t</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -131,6 +124,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>undeclared = w</t>
   </si>
 </sst>
 </file>
@@ -470,49 +466,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -526,84 +479,84 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -611,12 +564,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:F4"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,64 +577,64 @@
     <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -690,11 +643,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E4" sqref="E4:G4"/>
     </sheetView>
   </sheetViews>
@@ -706,123 +659,123 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Braga with everything switched on.
</commit_message>
<xml_diff>
--- a/Braga/Braga.xlsx
+++ b/Braga/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Relations" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Concept</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>v = w</t>
   </si>
   <si>
     <t>w</t>
@@ -466,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F8"/>
+      <selection activeCell="A6" sqref="A6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +474,7 @@
     <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,7 +485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -499,7 +496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -510,7 +507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -521,7 +518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -532,31 +529,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -566,10 +563,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +579,7 @@
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -593,7 +590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -604,7 +601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -615,26 +612,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +634,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G4"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
park mistakes, so Braga runs with no error messages
</commit_message>
<xml_diff>
--- a/Braga/Braga.xlsx
+++ b/Braga/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Relations" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>Concept</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>v = w</t>
   </si>
   <si>
     <t>w</t>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +477,7 @@
     <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -485,7 +488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -496,7 +499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -507,7 +510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -518,7 +521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -529,31 +532,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -563,9 +566,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
@@ -579,7 +582,7 @@
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -590,7 +593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -601,7 +604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -612,15 +615,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>